<commit_message>
definitive wg nb and committed of the submitted CR package
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_Geometry/CR_Geometry_WG_Numbers_table.xlsx
+++ b/publication/part1000/CR_Geometry/CR_Geometry_WG_Numbers_table.xlsx
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added 2 WG numbers for the CR
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_Geometry/CR_Geometry_WG_Numbers_table.xlsx
+++ b/publication/part1000/CR_Geometry/CR_Geometry_WG_Numbers_table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="136">
   <si>
     <t>Kevin Le Tutour</t>
   </si>
@@ -423,6 +423,18 @@
   </si>
   <si>
     <t>ISO 10303-1054 ed3 value_with_unit Document</t>
+  </si>
+  <si>
+    <t>N9213</t>
+  </si>
+  <si>
+    <t>N9214</t>
+  </si>
+  <si>
+    <t>CR_Geometry wg.number.publication_set</t>
+  </si>
+  <si>
+    <t>CR_Geometry wg.number.publication_set_comments</t>
   </si>
 </sst>
 </file>
@@ -780,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1835,6 +1847,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>